<commit_message>
Created new .jl to separate Provident run
</commit_message>
<xml_diff>
--- a/Cook County Project-C2C/results/Cook_County_results.xlsx
+++ b/Cook County Project-C2C/results/Cook_County_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbernal\Documents\GitHub\REopt_related_code\Cook County Project-C2C\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4F0D1C-5606-406D-8780-81D851A66BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5E05D6-53BC-4FDC-920E-E992CD223930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="21" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="29" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,11 @@
     <sheet name="ProvidentA_11" sheetId="28" r:id="rId28"/>
     <sheet name="CermakA_18" sheetId="29" r:id="rId29"/>
     <sheet name="MarkhamA_4" sheetId="30" r:id="rId30"/>
-    <sheet name="CermakA_19" r:id="rId34" sheetId="31"/>
-    <sheet name="MarkhamA_5" r:id="rId35" sheetId="32"/>
-    <sheet name="ProvdientA_2" r:id="rId36" sheetId="33"/>
+    <sheet name="CermakA_19" sheetId="31" r:id="rId31"/>
+    <sheet name="MarkhamA_5" sheetId="32" r:id="rId32"/>
+    <sheet name="ProvdientA_2" sheetId="33" r:id="rId33"/>
+    <sheet name="CermakA_20" r:id="rId37" sheetId="34"/>
+    <sheet name="MarkhamA_6" r:id="rId38" sheetId="35"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -542,7 +544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1CCC17-14D7-4D66-BC8D-DD8663B10AF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1EDFB6-003B-40D3-916A-4887B5533161}">
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -554,7 +556,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10272B7E-4F89-435D-93C4-8A0CF33D0D9E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8756D2-00F7-49A6-B485-9C8F37BF7F26}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -935,7 +937,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF13AFB-273F-439D-9595-5E13EFB7467F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB89762-FA85-40AA-93AB-3F1F2C6F2614}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1316,7 +1318,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E012F0-390D-4897-B237-4CE0E7A0181F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502B9D57-D36C-4348-808E-B7A02FBB9E82}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1697,7 +1699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B7139B-D2D1-4ABE-BA1A-F2DEDCB25DC1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EF35C8-05F2-4A34-887D-1D4B9F00E383}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2103,7 +2105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221D8A2C-41ED-411F-B338-51A8A50EABCE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180F6AB2-A78E-469B-A11D-ED155315C590}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2507,7 +2509,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646F245E-E83E-4EBA-B3A7-4B3620D2E2A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9DD933C-CFD5-46C3-9169-FC1CB9E35E29}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2912,7 +2914,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF486877-1F5F-4B4C-A437-9B52C4215B35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9AA68E-9590-45F3-A7F4-27FA5B180704}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3293,7 +3295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52602D4D-F299-472C-AB63-14637D78AE96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B94A597-7A5B-4908-A476-B75C6FC47E11}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3674,7 +3676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D939F298-9477-4D54-BE3C-0E156555AA9C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8DE4E0-CEE1-4A84-8AA7-61E11679A67C}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4055,7 +4057,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E186615-0987-4D37-9B2A-25313CBB2735}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1C6D17-56A6-4BA2-B722-DE11F5F206E1}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
@@ -4453,7 +4455,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7495CD5A-729E-426F-A992-19975BE302FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A938C5-C8E7-4878-8ECD-A83678743801}">
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5228,7 +5230,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C88CB5-C289-4EE8-91B3-A2D262E5B864}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C03F61E-B8D1-4747-98F5-1CC0561FAF83}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5609,7 +5611,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4688C147-FDE1-4E97-911E-CD1C8A9D454D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD938BB-57BA-45DD-AE00-99660DEACE24}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5990,7 +5992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFEE5820-F897-4A9A-84D7-6EC385E67ACA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46E5DF6-0883-4AF4-9352-8A8412CDD9C5}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6377,7 +6379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D5BD06-5749-4630-84BA-F2166A75C175}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB6C63A-2377-479B-8A9D-48F635E47E76}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6799,7 +6801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C01A6B4-8D42-4E15-8078-3B83305CA44A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEED5C59-9DC8-45AB-9765-B999BFCBECA3}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7196,7 +7198,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7631D23-3A2D-4B4C-9B09-557DE99E7C27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD98B9F5-5407-40D5-B7F3-BC7CE9C6C852}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0">
@@ -7615,7 +7617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC737FC0-38E9-4EEC-BBCB-2E38A08718FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D273866-75D1-405A-89B5-852C74CF1AB7}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8046,7 +8048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0653974D-B8DF-4C0E-B54F-F62E59D81248}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E0429B-BC45-441F-B020-B4077C5A6834}">
   <dimension ref="A1:AE18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8446,7 +8448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF4FE7C-7938-476B-AC78-7EBDE5CC47D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB01698-0FD7-4317-8279-AA5227B1E049}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8877,7 +8879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20094AAF-74BB-414B-A137-1F8048777FAA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C74EC0-CF53-40AA-BA70-6A11A835101A}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9306,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B819F569-9B23-4F7F-9BA4-D6C7403E4C62}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2E02C8-42F4-4C40-B0F8-663F071CBB48}">
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10067,10 +10069,10 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4066860-EFB2-4E92-91C7-D17563F2F3F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BB0FE2-231F-4657-BA92-FAB7737D10FE}">
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -10462,8 +10464,1259 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DA522B-6EB7-44F7-8AEB-EC6D625D6D56}">
+  <dimension ref="A1:AH4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:34" dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>33093</v>
+      </c>
+      <c r="D2">
+        <v>31631</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>227.185</v>
+      </c>
+      <c r="I2">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>31</v>
+      </c>
+      <c r="K2">
+        <v>503.09000000000003</v>
+      </c>
+      <c r="L2">
+        <v>30885</v>
+      </c>
+      <c r="M2">
+        <v>180.96</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>3011330</v>
+      </c>
+      <c r="Q2">
+        <v>968.53480000000002</v>
+      </c>
+      <c r="R2">
+        <v>968.53480000000002</v>
+      </c>
+      <c r="S2">
+        <v>974.76840000000004</v>
+      </c>
+      <c r="T2">
+        <v>24213.37</v>
+      </c>
+      <c r="U2">
+        <v>24369.21</v>
+      </c>
+      <c r="V2">
+        <v>0.01</v>
+      </c>
+      <c r="W2">
+        <v>160073.42000000001</v>
+      </c>
+      <c r="X2">
+        <v>19491.75</v>
+      </c>
+      <c r="Y2">
+        <v>249405.08</v>
+      </c>
+      <c r="Z2">
+        <v>171877.89</v>
+      </c>
+      <c r="AA2">
+        <v>337570.09</v>
+      </c>
+      <c r="AB2">
+        <v>50286.34</v>
+      </c>
+      <c r="AC2">
+        <v>616649.43000000005</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>31607.73</v>
+      </c>
+      <c r="AF2">
+        <v>0.01</v>
+      </c>
+      <c r="AG2">
+        <v>-144035.66</v>
+      </c>
+      <c r="AH2">
+        <v>6128591.6200000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>52158</v>
+      </c>
+      <c r="D3">
+        <v>49854</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>172.76300000000001</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>24</v>
+      </c>
+      <c r="K3">
+        <v>314.80599999999998</v>
+      </c>
+      <c r="L3">
+        <v>21608</v>
+      </c>
+      <c r="M3">
+        <v>190.75</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>2993088</v>
+      </c>
+      <c r="Q3">
+        <v>964.93679999999995</v>
+      </c>
+      <c r="R3">
+        <v>964.93679999999995</v>
+      </c>
+      <c r="S3">
+        <v>974.76840000000004</v>
+      </c>
+      <c r="T3">
+        <v>24123.42</v>
+      </c>
+      <c r="U3">
+        <v>24369.21</v>
+      </c>
+      <c r="V3">
+        <v>0.01</v>
+      </c>
+      <c r="W3">
+        <v>190890.6</v>
+      </c>
+      <c r="X3">
+        <v>13893.38</v>
+      </c>
+      <c r="Y3">
+        <v>304624.52</v>
+      </c>
+      <c r="Z3">
+        <v>199434.86</v>
+      </c>
+      <c r="AA3">
+        <v>335525.13</v>
+      </c>
+      <c r="AB3">
+        <v>50250.12</v>
+      </c>
+      <c r="AC3">
+        <v>614568.25</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>49836.5</v>
+      </c>
+      <c r="AF3">
+        <v>0.02</v>
+      </c>
+      <c r="AG3">
+        <v>-132257.9</v>
+      </c>
+      <c r="AH3">
+        <v>6138763.6900000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>52158</v>
+      </c>
+      <c r="D4">
+        <v>49854</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>149.19099999999997</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>24</v>
+      </c>
+      <c r="K4">
+        <v>314.80599999999998</v>
+      </c>
+      <c r="L4">
+        <v>21608</v>
+      </c>
+      <c r="M4">
+        <v>190.75</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>2993088</v>
+      </c>
+      <c r="Q4">
+        <v>964.93679999999995</v>
+      </c>
+      <c r="R4">
+        <v>964.93679999999995</v>
+      </c>
+      <c r="S4">
+        <v>974.76840000000004</v>
+      </c>
+      <c r="T4">
+        <v>24123.42</v>
+      </c>
+      <c r="U4">
+        <v>24369.21</v>
+      </c>
+      <c r="V4">
+        <v>0.01</v>
+      </c>
+      <c r="W4">
+        <v>190890.6</v>
+      </c>
+      <c r="X4">
+        <v>13893.38</v>
+      </c>
+      <c r="Y4">
+        <v>304624.52</v>
+      </c>
+      <c r="Z4">
+        <v>199434.86</v>
+      </c>
+      <c r="AA4">
+        <v>335525.13</v>
+      </c>
+      <c r="AB4">
+        <v>50250.12</v>
+      </c>
+      <c r="AC4">
+        <v>614568.25</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>49838.89</v>
+      </c>
+      <c r="AF4">
+        <v>0.02</v>
+      </c>
+      <c r="AG4">
+        <v>-113332.79</v>
+      </c>
+      <c r="AH4">
+        <v>6139196.1600000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36546FEB-7917-4111-9751-B9CF3FC6FA22}">
+  <dimension ref="A1:AE4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:31" dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>743</v>
+      </c>
+      <c r="C2">
+        <v>983520</v>
+      </c>
+      <c r="D2">
+        <v>940067</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>6677.9869999999992</v>
+      </c>
+      <c r="I2">
+        <v>355</v>
+      </c>
+      <c r="J2">
+        <v>1854</v>
+      </c>
+      <c r="K2">
+        <v>121686.20699999999</v>
+      </c>
+      <c r="L2">
+        <v>1167093.2</v>
+      </c>
+      <c r="M2">
+        <v>3632889</v>
+      </c>
+      <c r="N2">
+        <v>1092.1556</v>
+      </c>
+      <c r="O2">
+        <v>1092.1556</v>
+      </c>
+      <c r="P2">
+        <v>1066.8792000000001</v>
+      </c>
+      <c r="Q2">
+        <v>27303.89</v>
+      </c>
+      <c r="R2">
+        <v>26671.98</v>
+      </c>
+      <c r="S2">
+        <v>-0.02</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>815036.81</v>
+      </c>
+      <c r="V2">
+        <v>1167092.93</v>
+      </c>
+      <c r="W2">
+        <v>533740.25</v>
+      </c>
+      <c r="X2">
+        <v>423231.59</v>
+      </c>
+      <c r="Y2">
+        <v>100596.81</v>
+      </c>
+      <c r="Z2">
+        <v>543011.4</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>939389.34</v>
+      </c>
+      <c r="AC2">
+        <v>0.21</v>
+      </c>
+      <c r="AD2">
+        <v>-588084.67000000004</v>
+      </c>
+      <c r="AE2">
+        <v>6148985.2199999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>743</v>
+      </c>
+      <c r="C3">
+        <v>983520</v>
+      </c>
+      <c r="D3">
+        <v>940067</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>6002.05</v>
+      </c>
+      <c r="I3">
+        <v>411</v>
+      </c>
+      <c r="J3">
+        <v>2948</v>
+      </c>
+      <c r="K3">
+        <v>235258.19500000001</v>
+      </c>
+      <c r="L3">
+        <v>1715086.1</v>
+      </c>
+      <c r="M3">
+        <v>3645364</v>
+      </c>
+      <c r="N3">
+        <v>1116.6192000000001</v>
+      </c>
+      <c r="O3">
+        <v>1116.6192000000001</v>
+      </c>
+      <c r="P3">
+        <v>1066.8792000000001</v>
+      </c>
+      <c r="Q3">
+        <v>27915.48</v>
+      </c>
+      <c r="R3">
+        <v>26671.98</v>
+      </c>
+      <c r="S3">
+        <v>-0.05</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>1222716.67</v>
+      </c>
+      <c r="V3">
+        <v>1715090.56</v>
+      </c>
+      <c r="W3">
+        <v>812282.27</v>
+      </c>
+      <c r="X3">
+        <v>424684.94</v>
+      </c>
+      <c r="Y3">
+        <v>92913.73</v>
+      </c>
+      <c r="Z3">
+        <v>536781.67000000004</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>939457.91</v>
+      </c>
+      <c r="AC3">
+        <v>0.21</v>
+      </c>
+      <c r="AD3">
+        <v>-895593.18</v>
+      </c>
+      <c r="AE3">
+        <v>6496970.79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>743</v>
+      </c>
+      <c r="C4">
+        <v>983520</v>
+      </c>
+      <c r="D4">
+        <v>940067</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>4931.8719999999994</v>
+      </c>
+      <c r="I4">
+        <v>411</v>
+      </c>
+      <c r="J4">
+        <v>4414</v>
+      </c>
+      <c r="K4">
+        <v>372791.924</v>
+      </c>
+      <c r="L4">
+        <v>2381783.9500000002</v>
+      </c>
+      <c r="M4">
+        <v>3660427</v>
+      </c>
+      <c r="N4">
+        <v>1149.0627999999999</v>
+      </c>
+      <c r="O4">
+        <v>1149.0627999999999</v>
+      </c>
+      <c r="P4">
+        <v>1066.8792000000001</v>
+      </c>
+      <c r="Q4">
+        <v>28726.57</v>
+      </c>
+      <c r="R4">
+        <v>26671.98</v>
+      </c>
+      <c r="S4">
+        <v>-0.08</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>1733705.7</v>
+      </c>
+      <c r="V4">
+        <v>2381785.35</v>
+      </c>
+      <c r="W4">
+        <v>1167928.93</v>
+      </c>
+      <c r="X4">
+        <v>426439.74</v>
+      </c>
+      <c r="Y4">
+        <v>85792.7</v>
+      </c>
+      <c r="Z4">
+        <v>531415.43999999994</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>939566.47</v>
+      </c>
+      <c r="AC4">
+        <v>0.21</v>
+      </c>
+      <c r="AD4">
+        <v>-1336155.71</v>
+      </c>
+      <c r="AE4">
+        <v>6956539.7300000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A9EF7D-1E58-46AB-BB89-34AB7F3EB371}">
+  <dimension ref="A1:AH4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:34" dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>38</v>
+      </c>
+      <c r="C2">
+        <v>50639</v>
+      </c>
+      <c r="D2">
+        <v>48402</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>65.358000000000004</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>13</v>
+      </c>
+      <c r="K2">
+        <v>154.42600000000002</v>
+      </c>
+      <c r="L2">
+        <v>14496</v>
+      </c>
+      <c r="M2">
+        <v>11323322</v>
+      </c>
+      <c r="N2">
+        <v>808</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>3631.5468000000001</v>
+      </c>
+      <c r="R2">
+        <v>3631.5468000000001</v>
+      </c>
+      <c r="S2">
+        <v>3641.0904</v>
+      </c>
+      <c r="T2">
+        <v>90788.67</v>
+      </c>
+      <c r="U2">
+        <v>91027.26</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>590306.34</v>
+      </c>
+      <c r="X2">
+        <v>8963.7099999999991</v>
+      </c>
+      <c r="Y2">
+        <v>694245.1</v>
+      </c>
+      <c r="Z2">
+        <v>595639.43000000005</v>
+      </c>
+      <c r="AA2">
+        <v>1319167.04</v>
+      </c>
+      <c r="AB2">
+        <v>220602.28</v>
+      </c>
+      <c r="AC2">
+        <v>1558952.32</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>48395.35</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>-601719.55000000005</v>
+      </c>
+      <c r="AH2">
+        <v>15703993.52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>38</v>
+      </c>
+      <c r="C3">
+        <v>50639</v>
+      </c>
+      <c r="D3">
+        <v>48402</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>75.307000000000002</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>154.42600000000002</v>
+      </c>
+      <c r="L3">
+        <v>14496</v>
+      </c>
+      <c r="M3">
+        <v>11323322</v>
+      </c>
+      <c r="N3">
+        <v>869</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>3631.5468000000001</v>
+      </c>
+      <c r="R3">
+        <v>3631.5468000000001</v>
+      </c>
+      <c r="S3">
+        <v>3641.0904</v>
+      </c>
+      <c r="T3">
+        <v>90788.67</v>
+      </c>
+      <c r="U3">
+        <v>91027.26</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>629582.59</v>
+      </c>
+      <c r="X3">
+        <v>8963.7099999999991</v>
+      </c>
+      <c r="Y3">
+        <v>733521.35</v>
+      </c>
+      <c r="Z3">
+        <v>634915.68000000005</v>
+      </c>
+      <c r="AA3">
+        <v>1319167.04</v>
+      </c>
+      <c r="AB3">
+        <v>220602.28</v>
+      </c>
+      <c r="AC3">
+        <v>1558952.32</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>48394.34</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>-566729.71</v>
+      </c>
+      <c r="AH3">
+        <v>15757096.460000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>38</v>
+      </c>
+      <c r="C4">
+        <v>50639</v>
+      </c>
+      <c r="D4">
+        <v>48402</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>70.024000000000001</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>13</v>
+      </c>
+      <c r="K4">
+        <v>154.42600000000002</v>
+      </c>
+      <c r="L4">
+        <v>14496</v>
+      </c>
+      <c r="M4">
+        <v>11323322</v>
+      </c>
+      <c r="N4">
+        <v>869</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>3631.5468000000001</v>
+      </c>
+      <c r="R4">
+        <v>3631.5468000000001</v>
+      </c>
+      <c r="S4">
+        <v>3641.0904</v>
+      </c>
+      <c r="T4">
+        <v>90788.67</v>
+      </c>
+      <c r="U4">
+        <v>91027.26</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>629582.59</v>
+      </c>
+      <c r="X4">
+        <v>8963.7099999999991</v>
+      </c>
+      <c r="Y4">
+        <v>733521.35</v>
+      </c>
+      <c r="Z4">
+        <v>634915.68000000005</v>
+      </c>
+      <c r="AA4">
+        <v>1319167.04</v>
+      </c>
+      <c r="AB4">
+        <v>220602.28</v>
+      </c>
+      <c r="AC4">
+        <v>1558952.32</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>48394.87</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>-484663.97</v>
+      </c>
+      <c r="AH4">
+        <v>15759016.710000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:AH4"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -10584,7 +11837,7 @@
         <v>33093.0</v>
       </c>
       <c r="D2">
-        <v>31631.0</v>
+        <v>31540.0</v>
       </c>
       <c r="E2">
         <v>0.0</v>
@@ -10596,22 +11849,22 @@
         <v>0.0</v>
       </c>
       <c r="H2">
-        <v>227.185</v>
+        <v>0.0</v>
       </c>
       <c r="I2">
-        <v>19.0</v>
+        <v>0.0</v>
       </c>
       <c r="J2">
-        <v>31.0</v>
+        <v>0.0</v>
       </c>
       <c r="K2">
-        <v>503.09000000000003</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>30885.0</v>
+        <v>0.0</v>
       </c>
       <c r="M2">
-        <v>180.96</v>
+        <v>600.0</v>
       </c>
       <c r="N2">
         <v>0.0</v>
@@ -10620,19 +11873,19 @@
         <v>0.0</v>
       </c>
       <c r="P2">
-        <v>3.01133e6</v>
+        <v>3.011373e6</v>
       </c>
       <c r="Q2">
-        <v>968.5348</v>
+        <v>968.5476</v>
       </c>
       <c r="R2">
-        <v>968.5348</v>
+        <v>968.5476</v>
       </c>
       <c r="S2">
         <v>974.7684</v>
       </c>
       <c r="T2">
-        <v>24213.37</v>
+        <v>24213.69</v>
       </c>
       <c r="U2">
         <v>24369.21</v>
@@ -10641,40 +11894,40 @@
         <v>0.01</v>
       </c>
       <c r="W2">
-        <v>160073.42</v>
+        <v>41313.56</v>
       </c>
       <c r="X2">
-        <v>19491.75</v>
+        <v>0.0</v>
       </c>
       <c r="Y2">
-        <v>249405.08</v>
+        <v>100900.0</v>
       </c>
       <c r="Z2">
-        <v>171877.89</v>
+        <v>41313.56</v>
       </c>
       <c r="AA2">
-        <v>337570.09</v>
+        <v>337574.96</v>
       </c>
       <c r="AB2">
-        <v>50286.34</v>
+        <v>51798.68</v>
       </c>
       <c r="AC2">
-        <v>616649.43</v>
+        <v>618166.64</v>
       </c>
       <c r="AD2">
         <v>-0.0</v>
       </c>
       <c r="AE2">
-        <v>31607.73</v>
+        <v>31540.23</v>
       </c>
       <c r="AF2">
         <v>0.01</v>
       </c>
       <c r="AG2">
-        <v>-144035.66</v>
+        <v>1393.69</v>
       </c>
       <c r="AH2">
-        <v>6.12859162e6</v>
+        <v>6.90199032e6</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -10682,13 +11935,13 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>39.0</v>
+        <v>25.0</v>
       </c>
       <c r="C3">
-        <v>52158.0</v>
+        <v>33093.0</v>
       </c>
       <c r="D3">
-        <v>49854.0</v>
+        <v>31540.0</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -10700,22 +11953,22 @@
         <v>0.0</v>
       </c>
       <c r="H3">
-        <v>172.763</v>
+        <v>0.0</v>
       </c>
       <c r="I3">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="J3">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="K3">
-        <v>314.806</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>21608.0</v>
+        <v>0.0</v>
       </c>
       <c r="M3">
-        <v>190.75</v>
+        <v>600.0</v>
       </c>
       <c r="N3">
         <v>0.0</v>
@@ -10724,19 +11977,19 @@
         <v>0.0</v>
       </c>
       <c r="P3">
-        <v>2.993088e6</v>
+        <v>3.011373e6</v>
       </c>
       <c r="Q3">
-        <v>964.9368</v>
+        <v>968.5476</v>
       </c>
       <c r="R3">
-        <v>964.9368</v>
+        <v>968.5476</v>
       </c>
       <c r="S3">
         <v>974.7684</v>
       </c>
       <c r="T3">
-        <v>24123.42</v>
+        <v>24213.69</v>
       </c>
       <c r="U3">
         <v>24369.21</v>
@@ -10745,40 +11998,40 @@
         <v>0.01</v>
       </c>
       <c r="W3">
-        <v>190890.6</v>
+        <v>41313.56</v>
       </c>
       <c r="X3">
-        <v>13893.38</v>
+        <v>0.0</v>
       </c>
       <c r="Y3">
-        <v>304624.52</v>
+        <v>100900.0</v>
       </c>
       <c r="Z3">
-        <v>199434.86</v>
+        <v>41313.56</v>
       </c>
       <c r="AA3">
-        <v>335525.13</v>
+        <v>337574.96</v>
       </c>
       <c r="AB3">
-        <v>50250.12</v>
+        <v>51798.68</v>
       </c>
       <c r="AC3">
-        <v>614568.25</v>
+        <v>618166.64</v>
       </c>
       <c r="AD3">
         <v>-0.0</v>
       </c>
       <c r="AE3">
-        <v>49836.5</v>
+        <v>31540.23</v>
       </c>
       <c r="AF3">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="AG3">
-        <v>-132257.9</v>
+        <v>1393.69</v>
       </c>
       <c r="AH3">
-        <v>6.13876369e6</v>
+        <v>6.90299404e6</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -10786,13 +12039,13 @@
         <v>22</v>
       </c>
       <c r="B4">
-        <v>39.0</v>
+        <v>25.0</v>
       </c>
       <c r="C4">
-        <v>52158.0</v>
+        <v>33093.0</v>
       </c>
       <c r="D4">
-        <v>49854.0</v>
+        <v>31540.0</v>
       </c>
       <c r="E4">
         <v>0.0</v>
@@ -10804,22 +12057,22 @@
         <v>0.0</v>
       </c>
       <c r="H4">
-        <v>149.19099999999997</v>
+        <v>0.0</v>
       </c>
       <c r="I4">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="J4">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="K4">
-        <v>314.806</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>21608.0</v>
+        <v>0.0</v>
       </c>
       <c r="M4">
-        <v>190.75</v>
+        <v>600.0</v>
       </c>
       <c r="N4">
         <v>0.0</v>
@@ -10828,19 +12081,19 @@
         <v>0.0</v>
       </c>
       <c r="P4">
-        <v>2.993088e6</v>
+        <v>3.011373e6</v>
       </c>
       <c r="Q4">
-        <v>964.9368</v>
+        <v>968.5476</v>
       </c>
       <c r="R4">
-        <v>964.9368</v>
+        <v>968.5476</v>
       </c>
       <c r="S4">
         <v>974.7684</v>
       </c>
       <c r="T4">
-        <v>24123.42</v>
+        <v>24213.69</v>
       </c>
       <c r="U4">
         <v>24369.21</v>
@@ -10849,40 +12102,352 @@
         <v>0.01</v>
       </c>
       <c r="W4">
-        <v>190890.6</v>
+        <v>41313.56</v>
       </c>
       <c r="X4">
-        <v>13893.38</v>
+        <v>0.0</v>
       </c>
       <c r="Y4">
-        <v>304624.52</v>
+        <v>100900.0</v>
       </c>
       <c r="Z4">
-        <v>199434.86</v>
+        <v>41313.56</v>
       </c>
       <c r="AA4">
-        <v>335525.13</v>
+        <v>337574.96</v>
       </c>
       <c r="AB4">
-        <v>50250.12</v>
+        <v>51798.68</v>
       </c>
       <c r="AC4">
-        <v>614568.25</v>
+        <v>618166.64</v>
       </c>
       <c r="AD4">
         <v>-0.0</v>
       </c>
       <c r="AE4">
-        <v>49838.89</v>
+        <v>31540.23</v>
       </c>
       <c r="AF4">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="AG4">
-        <v>-113332.79</v>
+        <v>1393.69</v>
       </c>
       <c r="AH4">
-        <v>6.13919616e6</v>
+        <v>6.90387922e6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>25.0</v>
+      </c>
+      <c r="C5">
+        <v>33093.0</v>
+      </c>
+      <c r="D5">
+        <v>31540.0</v>
+      </c>
+      <c r="E5">
+        <v>0.0</v>
+      </c>
+      <c r="F5">
+        <v>0.0</v>
+      </c>
+      <c r="G5">
+        <v>0.0</v>
+      </c>
+      <c r="H5">
+        <v>0.0</v>
+      </c>
+      <c r="I5">
+        <v>0.0</v>
+      </c>
+      <c r="J5">
+        <v>0.0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0.0</v>
+      </c>
+      <c r="M5">
+        <v>300.0</v>
+      </c>
+      <c r="N5">
+        <v>0.0</v>
+      </c>
+      <c r="O5">
+        <v>0.0</v>
+      </c>
+      <c r="P5">
+        <v>3.011373e6</v>
+      </c>
+      <c r="Q5">
+        <v>968.5476</v>
+      </c>
+      <c r="R5">
+        <v>968.5476</v>
+      </c>
+      <c r="S5">
+        <v>974.7684</v>
+      </c>
+      <c r="T5">
+        <v>24213.69</v>
+      </c>
+      <c r="U5">
+        <v>24369.21</v>
+      </c>
+      <c r="V5">
+        <v>0.01</v>
+      </c>
+      <c r="W5">
+        <v>41313.56</v>
+      </c>
+      <c r="X5">
+        <v>0.0</v>
+      </c>
+      <c r="Y5">
+        <v>100900.0</v>
+      </c>
+      <c r="Z5">
+        <v>41313.56</v>
+      </c>
+      <c r="AA5">
+        <v>337574.96</v>
+      </c>
+      <c r="AB5">
+        <v>51798.68</v>
+      </c>
+      <c r="AC5">
+        <v>618166.64</v>
+      </c>
+      <c r="AD5">
+        <v>-0.0</v>
+      </c>
+      <c r="AE5">
+        <v>31540.23</v>
+      </c>
+      <c r="AF5">
+        <v>0.01</v>
+      </c>
+      <c r="AG5">
+        <v>1393.69</v>
+      </c>
+      <c r="AH5">
+        <v>6.83059762e6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>25.0</v>
+      </c>
+      <c r="C6">
+        <v>33093.0</v>
+      </c>
+      <c r="D6">
+        <v>31540.0</v>
+      </c>
+      <c r="E6">
+        <v>0.0</v>
+      </c>
+      <c r="F6">
+        <v>0.0</v>
+      </c>
+      <c r="G6">
+        <v>0.0</v>
+      </c>
+      <c r="H6">
+        <v>0.0</v>
+      </c>
+      <c r="I6">
+        <v>0.0</v>
+      </c>
+      <c r="J6">
+        <v>0.0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0.0</v>
+      </c>
+      <c r="M6">
+        <v>300.0</v>
+      </c>
+      <c r="N6">
+        <v>0.0</v>
+      </c>
+      <c r="O6">
+        <v>0.0</v>
+      </c>
+      <c r="P6">
+        <v>3.011373e6</v>
+      </c>
+      <c r="Q6">
+        <v>968.5476</v>
+      </c>
+      <c r="R6">
+        <v>968.5476</v>
+      </c>
+      <c r="S6">
+        <v>974.7684</v>
+      </c>
+      <c r="T6">
+        <v>24213.69</v>
+      </c>
+      <c r="U6">
+        <v>24369.21</v>
+      </c>
+      <c r="V6">
+        <v>0.01</v>
+      </c>
+      <c r="W6">
+        <v>41313.56</v>
+      </c>
+      <c r="X6">
+        <v>0.0</v>
+      </c>
+      <c r="Y6">
+        <v>100900.0</v>
+      </c>
+      <c r="Z6">
+        <v>41313.56</v>
+      </c>
+      <c r="AA6">
+        <v>337574.96</v>
+      </c>
+      <c r="AB6">
+        <v>51798.68</v>
+      </c>
+      <c r="AC6">
+        <v>618166.64</v>
+      </c>
+      <c r="AD6">
+        <v>-0.0</v>
+      </c>
+      <c r="AE6">
+        <v>31540.23</v>
+      </c>
+      <c r="AF6">
+        <v>0.01</v>
+      </c>
+      <c r="AG6">
+        <v>1393.69</v>
+      </c>
+      <c r="AH6">
+        <v>6.83109948e6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>25.0</v>
+      </c>
+      <c r="C7">
+        <v>33093.0</v>
+      </c>
+      <c r="D7">
+        <v>31540.0</v>
+      </c>
+      <c r="E7">
+        <v>0.0</v>
+      </c>
+      <c r="F7">
+        <v>0.0</v>
+      </c>
+      <c r="G7">
+        <v>0.0</v>
+      </c>
+      <c r="H7">
+        <v>0.0</v>
+      </c>
+      <c r="I7">
+        <v>0.0</v>
+      </c>
+      <c r="J7">
+        <v>0.0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0.0</v>
+      </c>
+      <c r="M7">
+        <v>300.0</v>
+      </c>
+      <c r="N7">
+        <v>0.0</v>
+      </c>
+      <c r="O7">
+        <v>0.0</v>
+      </c>
+      <c r="P7">
+        <v>3.011373e6</v>
+      </c>
+      <c r="Q7">
+        <v>968.5476</v>
+      </c>
+      <c r="R7">
+        <v>968.5476</v>
+      </c>
+      <c r="S7">
+        <v>974.7684</v>
+      </c>
+      <c r="T7">
+        <v>24213.69</v>
+      </c>
+      <c r="U7">
+        <v>24369.21</v>
+      </c>
+      <c r="V7">
+        <v>0.01</v>
+      </c>
+      <c r="W7">
+        <v>41313.56</v>
+      </c>
+      <c r="X7">
+        <v>0.0</v>
+      </c>
+      <c r="Y7">
+        <v>100900.0</v>
+      </c>
+      <c r="Z7">
+        <v>41313.56</v>
+      </c>
+      <c r="AA7">
+        <v>337574.96</v>
+      </c>
+      <c r="AB7">
+        <v>51798.68</v>
+      </c>
+      <c r="AC7">
+        <v>618166.64</v>
+      </c>
+      <c r="AD7">
+        <v>-0.0</v>
+      </c>
+      <c r="AE7">
+        <v>31540.23</v>
+      </c>
+      <c r="AF7">
+        <v>0.01</v>
+      </c>
+      <c r="AG7">
+        <v>1393.69</v>
+      </c>
+      <c r="AH7">
+        <v>6.83154207e6</v>
       </c>
     </row>
   </sheetData>
@@ -10890,9 +12455,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -11004,7 +12569,7 @@
         <v>983520.0</v>
       </c>
       <c r="D2">
-        <v>940067.0</v>
+        <v>937376.0</v>
       </c>
       <c r="E2">
         <v>0.0</v>
@@ -11016,76 +12581,76 @@
         <v>0.0</v>
       </c>
       <c r="H2">
-        <v>6677.986999999999</v>
+        <v>5463.151</v>
       </c>
       <c r="I2">
-        <v>355.0</v>
+        <v>711.0</v>
       </c>
       <c r="J2">
-        <v>1854.0</v>
+        <v>3709.0</v>
       </c>
       <c r="K2">
-        <v>121686.207</v>
+        <v>311557.02300000004</v>
       </c>
       <c r="L2">
-        <v>1.1670932e6</v>
+        <v>2.3341864e6</v>
       </c>
       <c r="M2">
-        <v>3.632889e6</v>
+        <v>3.656428e6</v>
       </c>
       <c r="N2">
-        <v>1092.1556</v>
+        <v>1134.9116</v>
       </c>
       <c r="O2">
-        <v>1092.1556</v>
+        <v>1134.9116</v>
       </c>
       <c r="P2">
-        <v>1066.8792</v>
+        <v>1067.41</v>
       </c>
       <c r="Q2">
-        <v>27303.89</v>
+        <v>28372.79</v>
       </c>
       <c r="R2">
-        <v>26671.98</v>
+        <v>26685.25</v>
       </c>
       <c r="S2">
-        <v>-0.02</v>
+        <v>-0.06</v>
       </c>
       <c r="T2">
         <v>0.0</v>
       </c>
       <c r="U2">
-        <v>815036.81</v>
+        <v>1.71382079e6</v>
       </c>
       <c r="V2">
-        <v>1.16709293e6</v>
+        <v>2.33418586e6</v>
       </c>
       <c r="W2">
-        <v>533740.25</v>
+        <v>1.04103141e6</v>
       </c>
       <c r="X2">
-        <v>423231.59</v>
+        <v>425973.88</v>
       </c>
       <c r="Y2">
-        <v>100596.81</v>
+        <v>88944.96</v>
       </c>
       <c r="Z2">
-        <v>543011.4</v>
+        <v>534101.84</v>
       </c>
       <c r="AA2">
         <v>-0.0</v>
       </c>
       <c r="AB2">
-        <v>939389.34</v>
+        <v>936821.6</v>
       </c>
       <c r="AC2">
         <v>0.21</v>
       </c>
       <c r="AD2">
-        <v>-588084.67</v>
+        <v>-1.3292481e6</v>
       </c>
       <c r="AE2">
-        <v>6.14898522e6</v>
+        <v>7.67172322e6</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -11099,7 +12664,7 @@
         <v>983520.0</v>
       </c>
       <c r="D3">
-        <v>940067.0</v>
+        <v>937376.0</v>
       </c>
       <c r="E3">
         <v>0.0</v>
@@ -11111,76 +12676,76 @@
         <v>0.0</v>
       </c>
       <c r="H3">
-        <v>6002.05</v>
+        <v>8457.886</v>
       </c>
       <c r="I3">
-        <v>411.0</v>
+        <v>830.0</v>
       </c>
       <c r="J3">
-        <v>2948.0</v>
+        <v>7322.0</v>
       </c>
       <c r="K3">
-        <v>235258.195</v>
+        <v>489211.26</v>
       </c>
       <c r="L3">
-        <v>1.7150861e6</v>
+        <v>4.08669625e6</v>
       </c>
       <c r="M3">
-        <v>3.645364e6</v>
+        <v>3.67534e6</v>
       </c>
       <c r="N3">
-        <v>1116.6192</v>
+        <v>1171.766</v>
       </c>
       <c r="O3">
-        <v>1116.6192</v>
+        <v>1171.766</v>
       </c>
       <c r="P3">
-        <v>1066.8792</v>
+        <v>1067.41</v>
       </c>
       <c r="Q3">
-        <v>27915.48</v>
+        <v>29294.15</v>
       </c>
       <c r="R3">
-        <v>26671.98</v>
+        <v>26685.25</v>
       </c>
       <c r="S3">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="T3">
         <v>0.0</v>
       </c>
       <c r="U3">
-        <v>1.22271667e6</v>
+        <v>3.09108276e6</v>
       </c>
       <c r="V3">
-        <v>1.71509056e6</v>
+        <v>4.08669601e6</v>
       </c>
       <c r="W3">
-        <v>812282.27</v>
+        <v>1.92621057e6</v>
       </c>
       <c r="X3">
-        <v>424684.94</v>
+        <v>428177.16</v>
       </c>
       <c r="Y3">
-        <v>92913.73</v>
+        <v>80416.11</v>
       </c>
       <c r="Z3">
-        <v>536781.67</v>
+        <v>527776.27</v>
       </c>
       <c r="AA3">
         <v>-0.0</v>
       </c>
       <c r="AB3">
-        <v>939457.91</v>
+        <v>936517.81</v>
       </c>
       <c r="AC3">
         <v>0.21</v>
       </c>
       <c r="AD3">
-        <v>-895593.18</v>
+        <v>-2.5460817e6</v>
       </c>
       <c r="AE3">
-        <v>6.49697079e6</v>
+        <v>8.98029686e6</v>
       </c>
     </row>
     <row r="4" spans="1:31">
@@ -11194,7 +12759,7 @@
         <v>983520.0</v>
       </c>
       <c r="D4">
-        <v>940067.0</v>
+        <v>937376.0</v>
       </c>
       <c r="E4">
         <v>0.0</v>
@@ -11206,505 +12771,361 @@
         <v>0.0</v>
       </c>
       <c r="H4">
-        <v>4931.871999999999</v>
+        <v>18277.023</v>
       </c>
       <c r="I4">
-        <v>411.0</v>
+        <v>830.0</v>
       </c>
       <c r="J4">
-        <v>4414.0</v>
+        <v>10437.0</v>
       </c>
       <c r="K4">
-        <v>372791.924</v>
+        <v>565568.032</v>
       </c>
       <c r="L4">
-        <v>2.38178395e6</v>
+        <v>5.5043261e6</v>
       </c>
       <c r="M4">
-        <v>3.660427e6</v>
+        <v>3.682974e6</v>
       </c>
       <c r="N4">
-        <v>1149.0628</v>
+        <v>1180.5832</v>
       </c>
       <c r="O4">
-        <v>1149.0628</v>
+        <v>1180.5832</v>
       </c>
       <c r="P4">
-        <v>1066.8792</v>
+        <v>1067.41</v>
       </c>
       <c r="Q4">
-        <v>28726.57</v>
+        <v>29514.58</v>
       </c>
       <c r="R4">
-        <v>26671.98</v>
+        <v>26685.25</v>
       </c>
       <c r="S4">
-        <v>-0.08</v>
+        <v>-0.11</v>
       </c>
       <c r="T4">
         <v>0.0</v>
       </c>
       <c r="U4">
-        <v>1.7337057e6</v>
+        <v>4.22626276e6</v>
       </c>
       <c r="V4">
-        <v>2.38178535e6</v>
+        <v>5.50432621e6</v>
       </c>
       <c r="W4">
-        <v>1.16792893e6</v>
+        <v>2.66637835e6</v>
       </c>
       <c r="X4">
-        <v>426439.74</v>
+        <v>429066.52</v>
       </c>
       <c r="Y4">
-        <v>85792.7</v>
+        <v>77070.71</v>
       </c>
       <c r="Z4">
-        <v>531415.44</v>
+        <v>525320.23</v>
       </c>
       <c r="AA4">
         <v>-0.0</v>
       </c>
       <c r="AB4">
-        <v>939566.47</v>
+        <v>935521.76</v>
       </c>
       <c r="AC4">
         <v>0.21</v>
       </c>
       <c r="AD4">
-        <v>-1.33615571e6</v>
+        <v>-3.61151452e6</v>
       </c>
       <c r="AE4">
-        <v>6.95653973e6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:AH4"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:34">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" t="s">
-        <v>32</v>
-      </c>
-      <c r="X1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34">
-      <c r="A2" t="s">
+        <v>1.008880714e7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B2">
-        <v>38.0</v>
-      </c>
-      <c r="C2">
-        <v>50639.0</v>
-      </c>
-      <c r="D2">
-        <v>48402.0</v>
-      </c>
-      <c r="E2">
+      <c r="B5">
+        <v>743.0</v>
+      </c>
+      <c r="C5">
+        <v>983520.0</v>
+      </c>
+      <c r="D5">
+        <v>937376.0</v>
+      </c>
+      <c r="E5">
         <v>0.0</v>
       </c>
-      <c r="F2">
+      <c r="F5">
         <v>0.0</v>
       </c>
-      <c r="G2">
+      <c r="G5">
         <v>0.0</v>
       </c>
-      <c r="H2">
-        <v>65.358</v>
-      </c>
-      <c r="I2">
-        <v>10.0</v>
-      </c>
-      <c r="J2">
-        <v>13.0</v>
-      </c>
-      <c r="K2">
-        <v>154.42600000000002</v>
-      </c>
-      <c r="L2">
-        <v>14496.0</v>
-      </c>
-      <c r="M2">
-        <v>1.1323322e7</v>
-      </c>
-      <c r="N2">
-        <v>808.0</v>
-      </c>
-      <c r="O2">
+      <c r="H5">
+        <v>6678.348999999999</v>
+      </c>
+      <c r="I5">
+        <v>355.0</v>
+      </c>
+      <c r="J5">
+        <v>1854.0</v>
+      </c>
+      <c r="K5">
+        <v>121856.234</v>
+      </c>
+      <c r="L5">
+        <v>1.1670932e6</v>
+      </c>
+      <c r="M5">
+        <v>3.635599e6</v>
+      </c>
+      <c r="N5">
+        <v>1092.7448</v>
+      </c>
+      <c r="O5">
+        <v>1092.7448</v>
+      </c>
+      <c r="P5">
+        <v>1067.41</v>
+      </c>
+      <c r="Q5">
+        <v>27318.62</v>
+      </c>
+      <c r="R5">
+        <v>26685.25</v>
+      </c>
+      <c r="S5">
+        <v>-0.02</v>
+      </c>
+      <c r="T5">
         <v>0.0</v>
       </c>
-      <c r="P2">
+      <c r="U5">
+        <v>856910.39</v>
+      </c>
+      <c r="V5">
+        <v>1.16709293e6</v>
+      </c>
+      <c r="W5">
+        <v>520515.71</v>
+      </c>
+      <c r="X5">
+        <v>423547.33</v>
+      </c>
+      <c r="Y5">
+        <v>100681.77</v>
+      </c>
+      <c r="Z5">
+        <v>543412.1</v>
+      </c>
+      <c r="AA5">
+        <v>-0.0</v>
+      </c>
+      <c r="AB5">
+        <v>936698.33</v>
+      </c>
+      <c r="AC5">
+        <v>0.21</v>
+      </c>
+      <c r="AD5">
+        <v>-599229.49</v>
+      </c>
+      <c r="AE5">
+        <v>6.91591141e6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>743.0</v>
+      </c>
+      <c r="C6">
+        <v>983520.0</v>
+      </c>
+      <c r="D6">
+        <v>937376.0</v>
+      </c>
+      <c r="E6">
         <v>0.0</v>
       </c>
-      <c r="Q2">
-        <v>3631.5468</v>
-      </c>
-      <c r="R2">
-        <v>3631.5468</v>
-      </c>
-      <c r="S2">
-        <v>3641.0904</v>
-      </c>
-      <c r="T2">
-        <v>90788.67</v>
-      </c>
-      <c r="U2">
-        <v>91027.26</v>
-      </c>
-      <c r="V2">
+      <c r="F6">
         <v>0.0</v>
       </c>
-      <c r="W2">
-        <v>590306.34</v>
-      </c>
-      <c r="X2">
-        <v>8963.71</v>
-      </c>
-      <c r="Y2">
-        <v>694245.1</v>
-      </c>
-      <c r="Z2">
-        <v>595639.43</v>
-      </c>
-      <c r="AA2">
-        <v>1.31916704e6</v>
-      </c>
-      <c r="AB2">
-        <v>220602.28</v>
-      </c>
-      <c r="AC2">
-        <v>1.55895232e6</v>
-      </c>
-      <c r="AD2">
+      <c r="G6">
+        <v>0.0</v>
+      </c>
+      <c r="H6">
+        <v>5995.566000000001</v>
+      </c>
+      <c r="I6">
+        <v>411.0</v>
+      </c>
+      <c r="J6">
+        <v>2952.0</v>
+      </c>
+      <c r="K6">
+        <v>236015.402</v>
+      </c>
+      <c r="L6">
+        <v>1.71696525e6</v>
+      </c>
+      <c r="M6">
+        <v>3.648139e6</v>
+      </c>
+      <c r="N6">
+        <v>1117.3464</v>
+      </c>
+      <c r="O6">
+        <v>1117.3464</v>
+      </c>
+      <c r="P6">
+        <v>1067.41</v>
+      </c>
+      <c r="Q6">
+        <v>27933.66</v>
+      </c>
+      <c r="R6">
+        <v>26685.25</v>
+      </c>
+      <c r="S6">
+        <v>-0.05</v>
+      </c>
+      <c r="T6">
+        <v>0.0</v>
+      </c>
+      <c r="U6">
+        <v>1.28517019e6</v>
+      </c>
+      <c r="V6">
+        <v>1.71696449e6</v>
+      </c>
+      <c r="W6">
+        <v>793820.21</v>
+      </c>
+      <c r="X6">
+        <v>425008.25</v>
+      </c>
+      <c r="Y6">
+        <v>92962.36</v>
+      </c>
+      <c r="Z6">
+        <v>537153.61</v>
+      </c>
+      <c r="AA6">
         <v>-0.0</v>
       </c>
-      <c r="AE2">
-        <v>48395.35</v>
-      </c>
-      <c r="AF2">
+      <c r="AB6">
+        <v>936767.59</v>
+      </c>
+      <c r="AC6">
+        <v>0.21</v>
+      </c>
+      <c r="AD6">
+        <v>-913659.33</v>
+      </c>
+      <c r="AE6">
+        <v>7.27621127e6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>743.0</v>
+      </c>
+      <c r="C7">
+        <v>983520.0</v>
+      </c>
+      <c r="D7">
+        <v>937376.0</v>
+      </c>
+      <c r="E7">
         <v>0.0</v>
       </c>
-      <c r="AG2">
-        <v>-601719.55</v>
-      </c>
-      <c r="AH2">
-        <v>1.570399352e7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>38.0</v>
-      </c>
-      <c r="C3">
-        <v>50639.0</v>
-      </c>
-      <c r="D3">
-        <v>48402.0</v>
-      </c>
-      <c r="E3">
+      <c r="F7">
         <v>0.0</v>
       </c>
-      <c r="F3">
+      <c r="G7">
         <v>0.0</v>
       </c>
-      <c r="G3">
+      <c r="H7">
+        <v>4933.978</v>
+      </c>
+      <c r="I7">
+        <v>411.0</v>
+      </c>
+      <c r="J7">
+        <v>4418.0</v>
+      </c>
+      <c r="K7">
+        <v>373624.515</v>
+      </c>
+      <c r="L7">
+        <v>2.3838997e6</v>
+      </c>
+      <c r="M7">
+        <v>3.66321e6</v>
+      </c>
+      <c r="N7">
+        <v>1149.8216</v>
+      </c>
+      <c r="O7">
+        <v>1149.8216</v>
+      </c>
+      <c r="P7">
+        <v>1067.41</v>
+      </c>
+      <c r="Q7">
+        <v>28745.54</v>
+      </c>
+      <c r="R7">
+        <v>26685.25</v>
+      </c>
+      <c r="S7">
+        <v>-0.08</v>
+      </c>
+      <c r="T7">
         <v>0.0</v>
       </c>
-      <c r="H3">
-        <v>75.307</v>
-      </c>
-      <c r="I3">
-        <v>10.0</v>
-      </c>
-      <c r="J3">
-        <v>13.0</v>
-      </c>
-      <c r="K3">
-        <v>154.42600000000002</v>
-      </c>
-      <c r="L3">
-        <v>14496.0</v>
-      </c>
-      <c r="M3">
-        <v>1.1323322e7</v>
-      </c>
-      <c r="N3">
-        <v>869.0</v>
-      </c>
-      <c r="O3">
-        <v>0.0</v>
-      </c>
-      <c r="P3">
-        <v>0.0</v>
-      </c>
-      <c r="Q3">
-        <v>3631.5468</v>
-      </c>
-      <c r="R3">
-        <v>3631.5468</v>
-      </c>
-      <c r="S3">
-        <v>3641.0904</v>
-      </c>
-      <c r="T3">
-        <v>90788.67</v>
-      </c>
-      <c r="U3">
-        <v>91027.26</v>
-      </c>
-      <c r="V3">
-        <v>0.0</v>
-      </c>
-      <c r="W3">
-        <v>629582.59</v>
-      </c>
-      <c r="X3">
-        <v>8963.71</v>
-      </c>
-      <c r="Y3">
-        <v>733521.35</v>
-      </c>
-      <c r="Z3">
-        <v>634915.68</v>
-      </c>
-      <c r="AA3">
-        <v>1.31916704e6</v>
-      </c>
-      <c r="AB3">
-        <v>220602.28</v>
-      </c>
-      <c r="AC3">
-        <v>1.55895232e6</v>
-      </c>
-      <c r="AD3">
+      <c r="U7">
+        <v>1.81922453e6</v>
+      </c>
+      <c r="V7">
+        <v>2.38389974e6</v>
+      </c>
+      <c r="W7">
+        <v>1.14203794e6</v>
+      </c>
+      <c r="X7">
+        <v>426764.02</v>
+      </c>
+      <c r="Y7">
+        <v>85836.4</v>
+      </c>
+      <c r="Z7">
+        <v>531783.42</v>
+      </c>
+      <c r="AA7">
         <v>-0.0</v>
       </c>
-      <c r="AE3">
-        <v>48394.34</v>
-      </c>
-      <c r="AF3">
-        <v>0.0</v>
-      </c>
-      <c r="AG3">
-        <v>-566729.71</v>
-      </c>
-      <c r="AH3">
-        <v>1.575709646e7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>38.0</v>
-      </c>
-      <c r="C4">
-        <v>50639.0</v>
-      </c>
-      <c r="D4">
-        <v>48402.0</v>
-      </c>
-      <c r="E4">
-        <v>0.0</v>
-      </c>
-      <c r="F4">
-        <v>0.0</v>
-      </c>
-      <c r="G4">
-        <v>0.0</v>
-      </c>
-      <c r="H4">
-        <v>70.024</v>
-      </c>
-      <c r="I4">
-        <v>10.0</v>
-      </c>
-      <c r="J4">
-        <v>13.0</v>
-      </c>
-      <c r="K4">
-        <v>154.42600000000002</v>
-      </c>
-      <c r="L4">
-        <v>14496.0</v>
-      </c>
-      <c r="M4">
-        <v>1.1323322e7</v>
-      </c>
-      <c r="N4">
-        <v>869.0</v>
-      </c>
-      <c r="O4">
-        <v>0.0</v>
-      </c>
-      <c r="P4">
-        <v>0.0</v>
-      </c>
-      <c r="Q4">
-        <v>3631.5468</v>
-      </c>
-      <c r="R4">
-        <v>3631.5468</v>
-      </c>
-      <c r="S4">
-        <v>3641.0904</v>
-      </c>
-      <c r="T4">
-        <v>90788.67</v>
-      </c>
-      <c r="U4">
-        <v>91027.26</v>
-      </c>
-      <c r="V4">
-        <v>0.0</v>
-      </c>
-      <c r="W4">
-        <v>629582.59</v>
-      </c>
-      <c r="X4">
-        <v>8963.71</v>
-      </c>
-      <c r="Y4">
-        <v>733521.35</v>
-      </c>
-      <c r="Z4">
-        <v>634915.68</v>
-      </c>
-      <c r="AA4">
-        <v>1.31916704e6</v>
-      </c>
-      <c r="AB4">
-        <v>220602.28</v>
-      </c>
-      <c r="AC4">
-        <v>1.55895232e6</v>
-      </c>
-      <c r="AD4">
-        <v>-0.0</v>
-      </c>
-      <c r="AE4">
-        <v>48394.87</v>
-      </c>
-      <c r="AF4">
-        <v>0.0</v>
-      </c>
-      <c r="AG4">
-        <v>-484663.97</v>
-      </c>
-      <c r="AH4">
-        <v>1.575901671e7</v>
+      <c r="AB7">
+        <v>936875.28</v>
+      </c>
+      <c r="AC7">
+        <v>0.21</v>
+      </c>
+      <c r="AD7">
+        <v>-1.36786092e6</v>
+      </c>
+      <c r="AE7">
+        <v>7.7519516e6</v>
       </c>
     </row>
   </sheetData>
@@ -11713,7 +13134,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302FF9D4-3188-4892-9E56-3D854CA9A79A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47415CC8-1181-432D-AD34-636F8812F1A0}">
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12476,7 +13897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA2DB6B4-8272-45AB-973C-CC0B390E0A39}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416652BD-C394-49EA-88E3-8AA0BAD72BFD}">
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13237,7 +14658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F603744F-F068-43C4-BBF9-47A053CAA1D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE1A997-F314-4A62-89BA-4413EE3B277B}">
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14011,7 +15432,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2613A67B-BD10-45F0-8C80-E78184959700}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F425FA-15E7-4C39-B473-676C2EDD0394}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14576,7 +15997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89326CDB-1FF1-4FEC-AD86-B28961BFB3FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A06C230-A691-4BE2-840C-1A38F86E1857}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
@@ -15146,7 +16567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC494A4-779E-4B61-A2D7-C8CF6AFC5679}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362D4CF7-5479-47CB-BDF8-D1581255825C}">
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
updated ProvidentA.JSON "fuel avail"
</commit_message>
<xml_diff>
--- a/Cook County Project-C2C/results/Cook_County_results.xlsx
+++ b/Cook County Project-C2C/results/Cook_County_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbernal\Documents\GitHub\REopt_related_code\Cook County Project-C2C\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB553CF-A27F-4FF5-94F3-7D3B86CD577D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001CAB61-3107-4E30-8C94-D36F80D73B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="40" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="42" activeTab="46" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,6 +59,7 @@
     <sheet name="CermakA_21" sheetId="44" r:id="rId44"/>
     <sheet name="MarkhamA_7" sheetId="45" r:id="rId45"/>
     <sheet name="ProvdientA_16" sheetId="46" r:id="rId46"/>
+    <sheet name="ProvdientA_18" sheetId="48" r:id="rId47"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="83">
   <si>
     <t>City</t>
   </si>
@@ -329,7 +330,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -370,7 +371,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -381,8 +382,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -665,26 +665,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E029ECE-79B5-41A9-A69E-98F644945F0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C152913-CEF7-4791-B0AD-BD8965C813CD}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4235F51-86F0-4FF6-A095-F8EBA1B60257}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC70B5F9-A151-44FD-8220-D56F3DD75B29}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -776,7 +776,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -868,7 +868,7 @@
         <v>6529404.04</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -960,7 +960,7 @@
         <v>6877347.7800000003</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1058,14 +1058,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A39F35-9C3F-4850-A9E7-9E9480F7C392}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026C17E9-3276-4AA6-89D5-5FB62F7C74FF}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>6529404.04</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>6877347.7800000003</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1439,14 +1439,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA8CCAD-56CF-477B-88DA-32E19846EA47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E9D67F-4B70-42DF-B8A2-AF7F8A2C4B1F}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>6529404.04</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>6877347.7800000003</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1820,34 +1820,34 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62427E0E-C687-4DEB-B54C-EB529DB8F1BB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBE7C9E-741F-4544-852D-ECA1397B0323}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>6529404.04</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>6877347.7800000003</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>7270693.1299999999</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2226,32 +2226,32 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD867E0-E539-4AA5-811C-93D1348D6149}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D106F585-18A9-4B28-9A63-9B4177C1E732}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>6233671.2000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>6420739.9800000004</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>7152790.2599999998</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2630,33 +2630,33 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C803C1-5132-4259-BDFA-4AF3590D42CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D82DFD4-1908-4A05-8AFA-B2970BB5433A}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>17442687.25</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>19579566.420000002</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>21759024.399999999</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -3035,14 +3035,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83ABB588-9B21-419B-81A5-3A288B8EF6D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179C6039-219F-4E15-99E6-42828A752F2A}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>6529404.04</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>6877347.7800000003</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3416,14 +3416,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977908FA-30AE-4137-86EC-2623BE0FD2CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6ACBD16-350B-4D4D-9855-1242D1F6BF0B}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>6529404.04</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>6877347.7800000003</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3797,14 +3797,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC530C89-962B-4392-B376-816A06D206CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6665371-1D8D-463E-8CB8-94B05ED19BF8}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>6233671.2000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>6420739.9800000004</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -4178,31 +4178,31 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CA2A52-654B-455F-8965-94B51DAA3B28}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADD2037-C645-49B1-A397-618DFC13CD38}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="15" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>6529404.04</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>6957884.3399999999</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -4576,28 +4576,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC26B3E7-045A-4287-A837-8D492AC3F44E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1054A8BF-6A7A-41FF-AEB4-A86A09F52FBF}">
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T2" sqref="T2:T11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>6066885.0999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>6302123.3499999996</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>6730545.3099999996</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>7208110.2800000003</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>7707651.0199999996</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>8218469.9199999999</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>8737502.1999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>9264134.0899999999</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -5277,7 +5277,7 @@
         <v>9797407.0999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -5351,14 +5351,14 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F47B5954-1F6F-48CF-840B-E477B68A8512}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60B904C-C829-47B3-BAA7-50BF6D36BDD4}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>6529404.04</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>6957884.3399999999</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -5732,14 +5732,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA55DBA-11D8-49B7-9242-6649023FFFA0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E507D1-5ACF-4E7D-B782-2F40D9A8BBED}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -5923,7 +5923,7 @@
         <v>6529404.04</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>6957884.3399999999</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -6113,20 +6113,20 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE26EECB-FD39-4772-B74B-64394ED430F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B372B35-8166-48FE-BB94-4F2CA92F464D}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AD2" sqref="AD2:AD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>6128591.6200000001</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>6138763.6900000004</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -6500,19 +6500,19 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566DC402-6933-4A2F-B9F8-1469ABB4AF06}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0AAC75-36B4-43AD-B02C-AB06C158CD03}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>6128591.6200000001</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>6138763.6900000004</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -6922,30 +6922,30 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BED968-13D5-404B-97D1-4E3FC0903126}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E79510-0D32-4B9C-B85F-F5E61BD550D1}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="15" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>6691400.0899999999</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -7221,7 +7221,7 @@
         <v>6773209.0899999999</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -7319,16 +7319,16 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1058CC-1685-4ED5-8738-891ACFEBA9A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3816A94-FD07-4658-BDDD-FD79BBF66ABD}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>15703993.52</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -7631,7 +7631,7 @@
         <v>15757096.460000001</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -7738,16 +7738,16 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962F6B17-038E-489D-BE7B-FEA633EAF581}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90EA06C-406E-4B58-B5DC-E94053E133B4}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7851,7 +7851,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>6128591.6200000001</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>6138763.6900000004</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -8169,16 +8169,16 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC98C6C-4C86-4DEB-A90E-B0628EC59CAD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B913BD2-0C53-4A8B-B537-289FD506EC48}">
   <dimension ref="A1:AE18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8273,7 +8273,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>6691400.0899999999</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -8463,7 +8463,7 @@
         <v>6765433</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>6982397.9199999999</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18">
         <v>1486</v>
       </c>
@@ -8569,16 +8569,16 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB05C91-55EC-45C2-B52A-81A9AD1E4564}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6C27BC-1874-4E6F-9E11-06FD2107261C}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8682,7 +8682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -8786,7 +8786,7 @@
         <v>15703993.52</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -8890,7 +8890,7 @@
         <v>15757096.460000001</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -9000,14 +9000,14 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFFD198-3758-4B3F-BF4F-4EAFE5A005F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF81F6DC-FF66-4921-B274-F0E43A8C4CD4}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9111,7 +9111,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -9215,7 +9215,7 @@
         <v>6128591.6200000001</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -9319,7 +9319,7 @@
         <v>6138763.6900000004</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -9429,14 +9429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41963CC2-DD4C-433C-B142-DABC31A5D9C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43653EA-E907-4F77-9633-DDD682228F78}">
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9504,7 +9504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -9572,7 +9572,7 @@
         <v>6066885.0999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -9640,7 +9640,7 @@
         <v>6302123.3499999996</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -9708,7 +9708,7 @@
         <v>6730545.3099999996</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -9776,7 +9776,7 @@
         <v>7208110.2800000003</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>7707651.0199999996</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -9912,7 +9912,7 @@
         <v>8218469.9199999999</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -9980,7 +9980,7 @@
         <v>8737502.1999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -10048,7 +10048,7 @@
         <v>9264134.0899999999</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -10116,7 +10116,7 @@
         <v>9797407.0999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -10190,16 +10190,16 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBBD5BDA-F784-4715-883E-59FDCF97F847}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF1B43D-0040-405B-AD5F-099AAEE6A934}">
   <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10294,7 +10294,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -10389,7 +10389,7 @@
         <v>6148985.2199999997</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -10484,7 +10484,7 @@
         <v>6496970.79</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -10585,14 +10585,14 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25CEAAB-D6D7-4250-89E8-4C2EE5FF283F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D91CB8-616B-4658-987C-E088A119A559}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10696,7 +10696,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -10800,7 +10800,7 @@
         <v>6128591.6200000001</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -10904,7 +10904,7 @@
         <v>6138763.6900000004</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -11014,14 +11014,14 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8F5F68-E807-4D34-8649-EF45FC6CCE2D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493D0458-9AE4-4FB9-897C-FAE464C208BB}">
   <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11116,7 +11116,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -11211,7 +11211,7 @@
         <v>6148985.2199999997</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -11306,7 +11306,7 @@
         <v>6496970.79</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -11407,14 +11407,14 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727B0522-2E57-43C4-B8EF-20D4D2928301}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310A2AEB-CA9C-49E7-B1BF-7C80234DEC51}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11518,7 +11518,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -11622,7 +11622,7 @@
         <v>15703993.52</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -11726,7 +11726,7 @@
         <v>15757096.460000001</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -11836,14 +11836,14 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DFA0DBC-A752-4B2F-8D42-760A9CCF83F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E08B15-4532-41C5-BB10-6B5CA7277C50}">
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11947,7 +11947,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -12051,7 +12051,7 @@
         <v>6901990.3200000003</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>6902994.04</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -12259,7 +12259,7 @@
         <v>6903879.2199999997</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -12363,7 +12363,7 @@
         <v>6830597.6200000001</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -12467,7 +12467,7 @@
         <v>6831099.4800000004</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -12577,14 +12577,14 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F49E150E-0DE8-4499-9B88-AE93D53C4105}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DAAF9A-6E6A-4070-AA72-ECDC8516C91E}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12679,7 +12679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -12774,7 +12774,7 @@
         <v>7671723.2199999997</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -12869,7 +12869,7 @@
         <v>8980296.8599999994</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -12964,7 +12964,7 @@
         <v>10088807.140000001</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -13059,7 +13059,7 @@
         <v>6915911.4100000001</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -13154,7 +13154,7 @@
         <v>7276211.2699999996</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -13255,14 +13255,14 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9587E125-E244-498C-A364-58E8E8A3C271}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F0AD28-8588-469C-9628-06C3293FC44B}">
   <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13366,7 +13366,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -13470,7 +13470,7 @@
         <v>17513321.760000002</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -13574,7 +13574,7 @@
         <v>17517103.289999999</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -13678,7 +13678,7 @@
         <v>17691615.289999999</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -13782,7 +13782,7 @@
         <v>17714907.149999999</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -13892,20 +13892,20 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7401C0C-1D7C-418B-8B26-F82ED28100CD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F081017F-2A90-4DBB-B505-AF2D7D58A97D}">
   <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="33" max="33" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -14009,7 +14009,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -14113,7 +14113,7 @@
         <v>17513321.760000002</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -14217,7 +14217,7 @@
         <v>17517103.289999999</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -14321,7 +14321,7 @@
         <v>17691615.289999999</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -14425,7 +14425,7 @@
         <v>17714907.149999999</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -14535,16 +14535,16 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CE207F-2653-44A9-A73D-38B0FE9D1438}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE10687F-12A5-4082-85E1-2FC22C350043}">
   <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -14648,7 +14648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -14752,7 +14752,7 @@
         <v>17519583.649999999</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -14862,16 +14862,16 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B94799E-B355-4233-97B3-D1067B899F5E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BE6308-6872-47FE-AB3B-2525357FD6B2}">
   <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -14975,7 +14975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -15079,7 +15079,7 @@
         <v>17470945.239999998</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -15189,16 +15189,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4061AF54-32BA-4424-87B6-36ABCEAEF9ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFC54B7-8ACF-43EB-A5D1-CD34612C4E9A}">
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -15266,7 +15266,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -15334,7 +15334,7 @@
         <v>6066885.0999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -15402,7 +15402,7 @@
         <v>6302123.3499999996</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -15470,7 +15470,7 @@
         <v>6730545.3099999996</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -15538,7 +15538,7 @@
         <v>7208110.2800000003</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -15606,7 +15606,7 @@
         <v>7707651.0199999996</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -15674,7 +15674,7 @@
         <v>8218469.9199999999</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -15742,7 +15742,7 @@
         <v>8737502.1999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -15810,7 +15810,7 @@
         <v>9264134.0899999999</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -15878,7 +15878,7 @@
         <v>9797407.0999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -15952,16 +15952,16 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DE32D3-9D05-4AA4-AB1C-35D1938D14C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DCF2DD-4113-42CA-8A17-F65CC1A1C9E3}">
   <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -16065,7 +16065,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -16169,7 +16169,7 @@
         <v>17516361.43</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -16273,7 +16273,7 @@
         <v>17520220.23</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -16377,7 +16377,7 @@
         <v>17672486.899999999</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -16481,7 +16481,7 @@
         <v>17748957.43</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -16591,21 +16591,21 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EC8DFA-5887-487D-8762-30BA6BCFCCE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA5FE74-6BEF-4367-99E8-A2DCA487519E}">
   <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -16709,7 +16709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -16813,7 +16813,7 @@
         <v>17516361.43</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -16917,7 +16917,7 @@
         <v>17520220.23</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -17021,7 +17021,7 @@
         <v>17672486.899999999</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -17125,7 +17125,7 @@
         <v>17748957.43</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -17235,21 +17235,21 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1075F0-C9C2-4B26-A410-AA751C2C3884}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4F2D20-4407-4357-93EC-EC064C68B93E}">
   <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AH2" sqref="AH2:AH6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -17353,7 +17353,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -17457,7 +17457,7 @@
         <v>17516361.43</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -17561,7 +17561,7 @@
         <v>17520220.23</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -17665,7 +17665,7 @@
         <v>17728419.460000001</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -17769,7 +17769,7 @@
         <v>17804360.469999999</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -17879,16 +17879,16 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DA339B-7641-49F3-83A4-DEAED377A1DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1871D6E-A534-43EE-817C-B5F13D215C19}">
   <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -17992,7 +17992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -18096,7 +18096,7 @@
         <v>17516361.43</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -18200,7 +18200,7 @@
         <v>17520220.23</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -18304,7 +18304,7 @@
         <v>17728419.460000001</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -18408,7 +18408,7 @@
         <v>17804360.469999999</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -18518,29 +18518,29 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A0C2A6-B675-4719-B19F-29F09E9981F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C65215-78E1-47F3-B2E3-CA2191B4E05A}">
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -18644,7 +18644,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -18748,7 +18748,7 @@
         <v>6902010.3099999996</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -18852,7 +18852,7 @@
         <v>6903014.0300000003</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -18956,7 +18956,7 @@
         <v>6903899.21</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -19060,7 +19060,7 @@
         <v>7015658.4000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -19164,7 +19164,7 @@
         <v>7087616.8799999999</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -19274,25 +19274,25 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2E0660-00B0-4779-AE86-B649D8DF0A97}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D763B1-C8F5-4392-9589-B6D5AB277CE1}">
   <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -19387,7 +19387,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -19482,7 +19482,7 @@
         <v>7671723.2199999997</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -19577,7 +19577,7 @@
         <v>8980296.8599999994</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -19672,7 +19672,7 @@
         <v>10088807.140000001</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -19767,7 +19767,7 @@
         <v>6915911.4100000001</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -19862,7 +19862,7 @@
         <v>7276211.2699999996</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -19957,7 +19957,7 @@
         <v>7751951.5999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="S10" t="s">
         <v>48</v>
       </c>
@@ -19968,27 +19968,27 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCF002F-B261-43D1-8F87-E58699709868}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CEF16D-872F-4457-BFF3-DC1AD085D76E}">
   <dimension ref="A1:AH12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -20092,7 +20092,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -20105,7 +20105,7 @@
       <c r="D2" s="7">
         <v>165221</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2">
@@ -20196,7 +20196,7 @@
         <v>17516361.43</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -20209,7 +20209,7 @@
       <c r="D3" s="7">
         <v>165221</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3">
@@ -20300,7 +20300,7 @@
         <v>17520220.23</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -20313,7 +20313,7 @@
       <c r="D4" s="7">
         <v>165221</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4">
@@ -20404,7 +20404,7 @@
         <v>17672486.899999999</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -20417,7 +20417,7 @@
       <c r="D5" s="7">
         <v>165221</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5">
@@ -20508,7 +20508,7 @@
         <v>17748957.43</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -20521,7 +20521,7 @@
       <c r="D6" s="7">
         <v>165221</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6">
@@ -20612,9 +20612,757 @@
         <v>18087788.5</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="T12" t="s">
         <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D5BD03-8411-4B2C-9E3F-BC3E06983836}">
+  <dimension ref="A1:AH7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>131</v>
+      </c>
+      <c r="C2">
+        <v>173354</v>
+      </c>
+      <c r="D2">
+        <v>165221</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>13</v>
+      </c>
+      <c r="K2">
+        <v>145.352</v>
+      </c>
+      <c r="L2" s="8">
+        <v>15279</v>
+      </c>
+      <c r="M2">
+        <v>11206503</v>
+      </c>
+      <c r="N2">
+        <v>2192</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>3608.5056</v>
+      </c>
+      <c r="R2">
+        <v>3608.5056</v>
+      </c>
+      <c r="S2">
+        <v>3641.0904</v>
+      </c>
+      <c r="T2">
+        <v>90212.64</v>
+      </c>
+      <c r="U2">
+        <v>91027.26</v>
+      </c>
+      <c r="V2">
+        <v>0.01</v>
+      </c>
+      <c r="W2">
+        <v>216416.94</v>
+      </c>
+      <c r="X2">
+        <v>10022.34</v>
+      </c>
+      <c r="Y2">
+        <v>543831.26</v>
+      </c>
+      <c r="Z2">
+        <v>221863.89</v>
+      </c>
+      <c r="AA2">
+        <v>1261852.19</v>
+      </c>
+      <c r="AB2">
+        <v>203360.84</v>
+      </c>
+      <c r="AC2">
+        <v>1491610.03</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>165220.37</v>
+      </c>
+      <c r="AF2">
+        <v>0.01</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>16589.61</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>16973208.219999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>131</v>
+      </c>
+      <c r="C3">
+        <v>173354</v>
+      </c>
+      <c r="D3">
+        <v>165221</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>145.352</v>
+      </c>
+      <c r="L3" s="8">
+        <v>15279</v>
+      </c>
+      <c r="M3">
+        <v>11206503</v>
+      </c>
+      <c r="N3">
+        <v>2192</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>3608.5056</v>
+      </c>
+      <c r="R3">
+        <v>3608.5056</v>
+      </c>
+      <c r="S3">
+        <v>3641.0904</v>
+      </c>
+      <c r="T3">
+        <v>90212.64</v>
+      </c>
+      <c r="U3">
+        <v>91027.26</v>
+      </c>
+      <c r="V3">
+        <v>0.01</v>
+      </c>
+      <c r="W3">
+        <v>216416.94</v>
+      </c>
+      <c r="X3">
+        <v>10022.34</v>
+      </c>
+      <c r="Y3">
+        <v>543831.26</v>
+      </c>
+      <c r="Z3">
+        <v>221863.89</v>
+      </c>
+      <c r="AA3">
+        <v>1261852.19</v>
+      </c>
+      <c r="AB3">
+        <v>203360.84</v>
+      </c>
+      <c r="AC3">
+        <v>1491610.03</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>165220.37</v>
+      </c>
+      <c r="AF3">
+        <v>0.01</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>16737.68</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>16976579.699999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>131</v>
+      </c>
+      <c r="C4">
+        <v>173354</v>
+      </c>
+      <c r="D4">
+        <v>165221</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>13</v>
+      </c>
+      <c r="K4">
+        <v>145.352</v>
+      </c>
+      <c r="L4" s="8">
+        <v>15279</v>
+      </c>
+      <c r="M4">
+        <v>11206503</v>
+      </c>
+      <c r="N4">
+        <v>2192</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>3608.5056</v>
+      </c>
+      <c r="R4">
+        <v>3608.5056</v>
+      </c>
+      <c r="S4">
+        <v>3641.0904</v>
+      </c>
+      <c r="T4">
+        <v>90212.64</v>
+      </c>
+      <c r="U4">
+        <v>91027.26</v>
+      </c>
+      <c r="V4">
+        <v>0.01</v>
+      </c>
+      <c r="W4">
+        <v>216416.94</v>
+      </c>
+      <c r="X4">
+        <v>10022.34</v>
+      </c>
+      <c r="Y4">
+        <v>543831.26</v>
+      </c>
+      <c r="Z4">
+        <v>221863.89</v>
+      </c>
+      <c r="AA4">
+        <v>1261852.19</v>
+      </c>
+      <c r="AB4">
+        <v>203360.84</v>
+      </c>
+      <c r="AC4">
+        <v>1491610.03</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>165220.37</v>
+      </c>
+      <c r="AF4">
+        <v>0.01</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>16761.29</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>16977382.350000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>131</v>
+      </c>
+      <c r="C5">
+        <v>173354</v>
+      </c>
+      <c r="D5">
+        <v>165221</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>38</v>
+      </c>
+      <c r="J5">
+        <v>65</v>
+      </c>
+      <c r="K5">
+        <v>866.34300000000007</v>
+      </c>
+      <c r="L5" s="8">
+        <v>64551</v>
+      </c>
+      <c r="M5">
+        <v>11206568</v>
+      </c>
+      <c r="N5">
+        <v>1556</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>3608.5475999999999</v>
+      </c>
+      <c r="R5">
+        <v>3608.5475999999999</v>
+      </c>
+      <c r="S5">
+        <v>3641.0904</v>
+      </c>
+      <c r="T5">
+        <v>90213.69</v>
+      </c>
+      <c r="U5">
+        <v>91027.26</v>
+      </c>
+      <c r="V5">
+        <v>0.01</v>
+      </c>
+      <c r="W5">
+        <v>515444.57</v>
+      </c>
+      <c r="X5">
+        <v>43298.22</v>
+      </c>
+      <c r="Y5">
+        <v>892131.05</v>
+      </c>
+      <c r="Z5">
+        <v>539547.36</v>
+      </c>
+      <c r="AA5">
+        <v>1261859.51</v>
+      </c>
+      <c r="AB5">
+        <v>201118.71</v>
+      </c>
+      <c r="AC5">
+        <v>1489375.22</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>165220.37</v>
+      </c>
+      <c r="AF5">
+        <v>0.01</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>-345983.05</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>17130798.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>131</v>
+      </c>
+      <c r="C6">
+        <v>173354</v>
+      </c>
+      <c r="D6">
+        <v>165221</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>27</v>
+      </c>
+      <c r="J6">
+        <v>59</v>
+      </c>
+      <c r="K6">
+        <v>683.97</v>
+      </c>
+      <c r="L6" s="8">
+        <v>51056</v>
+      </c>
+      <c r="M6">
+        <v>11206549</v>
+      </c>
+      <c r="N6">
+        <v>1642</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>3608.5320000000002</v>
+      </c>
+      <c r="R6">
+        <v>3608.5320000000002</v>
+      </c>
+      <c r="S6">
+        <v>3641.0904</v>
+      </c>
+      <c r="T6">
+        <v>90213.3</v>
+      </c>
+      <c r="U6">
+        <v>91027.26</v>
+      </c>
+      <c r="V6">
+        <v>0.01</v>
+      </c>
+      <c r="W6">
+        <v>571206.56999999995</v>
+      </c>
+      <c r="X6">
+        <v>35056.5</v>
+      </c>
+      <c r="Y6">
+        <v>934400.78</v>
+      </c>
+      <c r="Z6">
+        <v>591196.51</v>
+      </c>
+      <c r="AA6">
+        <v>1261857.4099999999</v>
+      </c>
+      <c r="AB6">
+        <v>201547.04</v>
+      </c>
+      <c r="AC6">
+        <v>1489801.45</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>165220.37</v>
+      </c>
+      <c r="AF6">
+        <v>0.01</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>-348531.21</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>17206611.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>131</v>
+      </c>
+      <c r="C7">
+        <v>173354</v>
+      </c>
+      <c r="D7">
+        <v>165221</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>27</v>
+      </c>
+      <c r="J7">
+        <v>59</v>
+      </c>
+      <c r="K7">
+        <v>683.97</v>
+      </c>
+      <c r="L7" s="8">
+        <v>51056</v>
+      </c>
+      <c r="M7">
+        <v>11206549</v>
+      </c>
+      <c r="N7">
+        <v>1209</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>3608.5320000000002</v>
+      </c>
+      <c r="R7">
+        <v>3608.5320000000002</v>
+      </c>
+      <c r="S7">
+        <v>3641.0904</v>
+      </c>
+      <c r="T7">
+        <v>90213.3</v>
+      </c>
+      <c r="U7">
+        <v>91027.26</v>
+      </c>
+      <c r="V7">
+        <v>0.01</v>
+      </c>
+      <c r="W7">
+        <v>289629.65999999997</v>
+      </c>
+      <c r="X7">
+        <v>35056.5</v>
+      </c>
+      <c r="Y7">
+        <v>652823.87</v>
+      </c>
+      <c r="Z7">
+        <v>309619.59999999998</v>
+      </c>
+      <c r="AA7">
+        <v>1261857.4099999999</v>
+      </c>
+      <c r="AB7">
+        <v>201547.04</v>
+      </c>
+      <c r="AC7">
+        <v>1489801.45</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>165220.37</v>
+      </c>
+      <c r="AF7">
+        <v>0.01</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>-44810.32</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>16823368.73</v>
       </c>
     </row>
   </sheetData>
@@ -20623,14 +21371,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F129C13-B39C-4670-AFF6-2F5115340D6B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E88BE3-AE96-44FE-A5B5-BE8D150497F9}">
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -20698,7 +21446,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -20766,7 +21514,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -20834,7 +21582,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -20902,7 +21650,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -20970,7 +21718,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -21038,7 +21786,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -21106,7 +21854,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -21174,7 +21922,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -21242,7 +21990,7 @@
         <v>4754481.9800000004</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -21310,7 +22058,7 @@
         <v>5585958.5300000003</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -21384,19 +22132,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB05FF9-5AFA-4EAB-88DC-F4F06C4954FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378658D7-F134-485F-B5F4-6B213265FCC6}">
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -21464,7 +22212,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -21532,7 +22280,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -21600,7 +22348,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -21668,7 +22416,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -21736,7 +22484,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -21804,7 +22552,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -21872,7 +22620,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -21940,7 +22688,7 @@
         <v>4411760.7300000004</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -22008,7 +22756,7 @@
         <v>4754481.9800000004</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -22076,7 +22824,7 @@
         <v>5585958.5300000003</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -22144,10 +22892,10 @@
         <v>6628685.9699999997</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -22158,14 +22906,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2E18E0-0705-47D9-B99B-840FF49A6DCA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED8B67F-C9B4-4E2A-9373-14CB33959BD1}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -22257,7 +23005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -22349,7 +23097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -22441,7 +23189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -22533,7 +23281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -22625,7 +23373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -22723,19 +23471,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6509DAFF-243B-4D6E-9674-A63516B78831}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F7CB8D-B345-4EB8-B50B-5C5517B06CEC}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="28" max="28" width="10.85546875" style="5"/>
+    <col min="28" max="28" width="10.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -22827,7 +23575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -22919,7 +23667,7 @@
         <v>7861753.04</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -23011,7 +23759,7 @@
         <v>7861753.04</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -23103,7 +23851,7 @@
         <v>8569721.6500000004</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -23195,7 +23943,7 @@
         <v>11319914.380000001</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -23293,19 +24041,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71FB0F3-2930-45C5-9EA0-BF6AD27854F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCD0FFF-AC02-4D46-868C-1343A77D4272}">
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="U2" sqref="U2:U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -23373,7 +24121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -23441,7 +24189,7 @@
         <v>6136332.8399999999</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -23509,7 +24257,7 @@
         <v>6394248.5499999998</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -23577,7 +24325,7 @@
         <v>6531112.8600000003</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -23645,7 +24393,7 @@
         <v>6732116.8099999996</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -23713,7 +24461,7 @@
         <v>6933297.8200000003</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -23781,7 +24529,7 @@
         <v>7134587.9800000004</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -23849,7 +24597,7 @@
         <v>7698932.6399999997</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -23917,7 +24665,7 @@
         <v>8423445.5</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -23985,7 +24733,7 @@
         <v>9202458.9600000009</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>

</xml_diff>